<commit_message>
Joined xml objects with java code, Added permissions, Started authentication.
</commit_message>
<xml_diff>
--- a/RookiePLays/Moview_progress report.xlsx
+++ b/RookiePLays/Moview_progress report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali\Documents\RookiePLays\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali\Documents\recycler-view-search-master\Moview2\Moview\RookiePLays\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{678A5238-0CE5-4DAA-A3D8-C4B4ADA1ADDD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{10E9B601-3BEC-4DCE-94CE-7680F7AB3F49}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11712" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -387,6 +387,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="6" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="6" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="5" xfId="3" applyNumberFormat="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="3">
       <alignment horizontal="left"/>
     </xf>
@@ -397,9 +400,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="14" fontId="4" fillId="2" borderId="5" xfId="3" applyNumberFormat="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Date" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1075,8 +1075,8 @@
   </sheetPr>
   <dimension ref="B1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1100,33 +1100,33 @@
     </row>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="24" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21">
+      <c r="C4" s="23"/>
+      <c r="D4" s="22">
         <v>43252</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
@@ -1144,7 +1144,7 @@
     </row>
     <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1318,33 +1318,33 @@
     </row>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
@@ -1524,33 +1524,33 @@
     </row>
     <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="20"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="23"/>
+      <c r="D4" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="22"/>
     </row>
     <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">

</xml_diff>